<commit_message>
Doing analysis again with logs in new places
</commit_message>
<xml_diff>
--- a/class/hit_miss.xlsx
+++ b/class/hit_miss.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-16020" yWindow="-19780" windowWidth="25600" windowHeight="16980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-16020" yWindow="-19780" windowWidth="25600" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="hit_miss.csv" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="v1" sheetId="2" r:id="rId2"/>
+    <sheet name="v3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="hit_miss" localSheetId="1">Sheet1!$A$1:$C$27</definedName>
+    <definedName name="hit_miss" localSheetId="1">'v1'!$A$1:$C$27</definedName>
+    <definedName name="hit_miss" localSheetId="2">'v3'!$A$1:$C$28</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -26,6 +28,15 @@
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="hit_miss.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:nathanwoods:workspaces:go:src:github.com:bign8:cdn:class:v2:hit_miss.csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="hit_miss.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:nathanwoods:workspaces:go:src:github.com:bign8:cdn:class:v3:hit_miss.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -52,10 +63,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +112,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -140,10 +187,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>hit_miss.csv!$A$2:$A$29</c:f>
+              <c:f>hit_miss.csv!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -221,105 +268,93 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>57.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>hit_miss.csv!$D$2:$D$29</c:f>
+              <c:f>hit_miss.csv!$D$2:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0.878723404255319</c:v>
+                  <c:v>1.985436893203883</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96821008984105</c:v>
+                  <c:v>2.806295399515739</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.08582638548308</c:v>
+                  <c:v>3.201820940819423</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.149480968858132</c:v>
+                  <c:v>2.692599620493358</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.242189739180281</c:v>
+                  <c:v>2.74370709382151</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.361708065866592</c:v>
+                  <c:v>2.838383838383838</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.369531074713933</c:v>
+                  <c:v>3.413814180929095</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.421895609572263</c:v>
+                  <c:v>3.251014198782961</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.365873666940115</c:v>
+                  <c:v>3.695588235294118</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.561510974987238</c:v>
+                  <c:v>4.245395719263314</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.486230381995854</c:v>
+                  <c:v>3.610629921259842</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.572842381021685</c:v>
+                  <c:v>3.697478991596639</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.560524381279098</c:v>
+                  <c:v>4.098181818181819</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.580211214483279</c:v>
+                  <c:v>4.488999290276792</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.601497504159734</c:v>
+                  <c:v>3.870977443609023</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.727272727272727</c:v>
+                  <c:v>4.144689737470167</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.675248993430812</c:v>
+                  <c:v>4.711946634323832</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.750918056867065</c:v>
+                  <c:v>5.067301782421634</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.83347124534547</c:v>
+                  <c:v>6.531794095382285</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.879741186970103</c:v>
+                  <c:v>5.014693651233713</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.804830287206266</c:v>
+                  <c:v>6.555704697986577</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.821840575938937</c:v>
+                  <c:v>5.584039355015031</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.852241085062427</c:v>
+                  <c:v>6.359285065131778</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.021970510692315</c:v>
+                  <c:v>7.552889489692464</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.019063483250046</c:v>
+                  <c:v>6.587375803623612</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.91474912112496</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.121422060164084</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.18883440211241</c:v>
+                  <c:v>6.782283577796951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -336,11 +371,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2108428600"/>
-        <c:axId val="-2108436680"/>
+        <c:axId val="-2077937896"/>
+        <c:axId val="-2077658680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2108428600"/>
+        <c:axId val="-2077937896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -374,7 +409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108436680"/>
+        <c:crossAx val="-2077658680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -382,7 +417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108436680"/>
+        <c:axId val="-2077658680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,7 +447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108428600"/>
+        <c:crossAx val="-2077937896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -492,10 +527,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>hit_miss.csv!$A$2:$A$29</c:f>
+              <c:f>hit_miss.csv!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -573,105 +608,93 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>57.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>hit_miss.csv!$B$2:$B$29</c:f>
+              <c:f>hit_miss.csv!$B$2:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>413.0</c:v>
+                  <c:v>409.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1401.0</c:v>
+                  <c:v>1159.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2214.0</c:v>
+                  <c:v>2110.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3322.0</c:v>
+                  <c:v>2838.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4334.0</c:v>
+                  <c:v>3597.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4879.0</c:v>
+                  <c:v>4496.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6104.0</c:v>
+                  <c:v>5585.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7546.0</c:v>
+                  <c:v>6411.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8325.0</c:v>
+                  <c:v>7539.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9177.0</c:v>
+                  <c:v>8529.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10038.0</c:v>
+                  <c:v>9171.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10807.0</c:v>
+                  <c:v>10120.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12737.0</c:v>
+                  <c:v>11270.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12569.0</c:v>
+                  <c:v>12650.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13475.0</c:v>
+                  <c:v>12871.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14079.0</c:v>
+                  <c:v>13893.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15811.0</c:v>
+                  <c:v>15540.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16688.0</c:v>
+                  <c:v>16489.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17726.0</c:v>
+                  <c:v>17257.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16850.0</c:v>
+                  <c:v>18088.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19355.0</c:v>
+                  <c:v>19536.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21004.0</c:v>
+                  <c:v>20432.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20621.0</c:v>
+                  <c:v>20992.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>20707.0</c:v>
+                  <c:v>22349.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>21818.0</c:v>
+                  <c:v>22542.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23965.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>23272.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>29013.0</c:v>
+                  <c:v>23582.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -697,10 +720,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>hit_miss.csv!$A$2:$A$29</c:f>
+              <c:f>hit_miss.csv!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -778,105 +801,93 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>57.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>hit_miss.csv!$C$2:$C$29</c:f>
+              <c:f>hit_miss.csv!$C$2:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>470.0</c:v>
+                  <c:v>206.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1447.0</c:v>
+                  <c:v>413.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2039.0</c:v>
+                  <c:v>659.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2890.0</c:v>
+                  <c:v>1054.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3489.0</c:v>
+                  <c:v>1311.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3583.0</c:v>
+                  <c:v>1584.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4457.0</c:v>
+                  <c:v>1636.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5307.0</c:v>
+                  <c:v>1972.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6095.0</c:v>
+                  <c:v>2040.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5877.0</c:v>
+                  <c:v>2009.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6754.0</c:v>
+                  <c:v>2540.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6871.0</c:v>
+                  <c:v>2737.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8162.0</c:v>
+                  <c:v>2750.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7954.0</c:v>
+                  <c:v>2818.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8414.0</c:v>
+                  <c:v>3325.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8151.0</c:v>
+                  <c:v>3352.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9438.0</c:v>
+                  <c:v>3298.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9531.0</c:v>
+                  <c:v>3254.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9668.0</c:v>
+                  <c:v>2642.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8964.0</c:v>
+                  <c:v>3607.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10724.0</c:v>
+                  <c:v>2980.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11529.0</c:v>
+                  <c:v>3659.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11133.0</c:v>
+                  <c:v>3301.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10241.0</c:v>
+                  <c:v>2959.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10806.0</c:v>
+                  <c:v>3422.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12516.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10970.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>13255.0</c:v>
+                  <c:v>3477.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -893,11 +904,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2087215880"/>
-        <c:axId val="-2108074200"/>
+        <c:axId val="-2077977080"/>
+        <c:axId val="-2077971320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087215880"/>
+        <c:axId val="-2077977080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108074200"/>
+        <c:crossAx val="-2077971320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -939,7 +950,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108074200"/>
+        <c:axId val="-2077971320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,7 +985,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087215880"/>
+        <c:crossAx val="-2077977080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1030,16 +1041,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1063,6 +1074,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hit_miss" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="hit_miss" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1387,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1407,423 +1422,393 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>413</v>
-      </c>
-      <c r="C2">
-        <v>470</v>
+      <c r="B2" s="1">
+        <v>409</v>
+      </c>
+      <c r="C2" s="1">
+        <v>206</v>
       </c>
       <c r="D2">
         <f>B2/C2</f>
-        <v>0.87872340425531914</v>
+        <v>1.9854368932038835</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1401</v>
-      </c>
-      <c r="C3">
-        <v>1447</v>
+      <c r="B3" s="1">
+        <v>1159</v>
+      </c>
+      <c r="C3" s="1">
+        <v>413</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D29" si="0">B3/C3</f>
-        <v>0.9682100898410505</v>
+        <f t="shared" ref="D3:D27" si="0">B3/C3</f>
+        <v>2.8062953995157387</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>2214</v>
-      </c>
-      <c r="C4">
-        <v>2039</v>
+      <c r="B4" s="1">
+        <v>2110</v>
+      </c>
+      <c r="C4" s="1">
+        <v>659</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1.0858263854830799</v>
+        <v>3.2018209408194234</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>3322</v>
-      </c>
-      <c r="C5">
-        <v>2890</v>
+      <c r="B5" s="1">
+        <v>2838</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1054</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1.1494809688581316</v>
+        <v>2.6925996204933584</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>4334</v>
-      </c>
-      <c r="C6">
-        <v>3489</v>
+      <c r="B6" s="1">
+        <v>3597</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1311</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1.242189739180281</v>
+        <v>2.7437070938215102</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>4879</v>
-      </c>
-      <c r="C7">
-        <v>3583</v>
+      <c r="B7" s="1">
+        <v>4496</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1584</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1.3617080658665923</v>
+        <v>2.8383838383838382</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>6104</v>
-      </c>
-      <c r="C8">
-        <v>4457</v>
+      <c r="B8" s="1">
+        <v>5585</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1636</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>1.3695310747139331</v>
+        <v>3.4138141809290952</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>15</v>
       </c>
-      <c r="B9">
-        <v>7546</v>
-      </c>
-      <c r="C9">
-        <v>5307</v>
+      <c r="B9" s="1">
+        <v>6411</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1972</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1.421895609572263</v>
+        <v>3.2510141987829613</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>17</v>
       </c>
-      <c r="B10">
-        <v>8325</v>
-      </c>
-      <c r="C10">
-        <v>6095</v>
+      <c r="B10" s="1">
+        <v>7539</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2040</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>1.3658736669401148</v>
+        <v>3.6955882352941178</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>19</v>
       </c>
-      <c r="B11">
-        <v>9177</v>
-      </c>
-      <c r="C11">
-        <v>5877</v>
+      <c r="B11" s="1">
+        <v>8529</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2009</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>1.5615109749872385</v>
+        <v>4.2453957192633149</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>21</v>
       </c>
-      <c r="B12">
-        <v>10038</v>
-      </c>
-      <c r="C12">
-        <v>6754</v>
+      <c r="B12" s="1">
+        <v>9171</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2540</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>1.4862303819958542</v>
+        <v>3.6106299212598425</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>23</v>
       </c>
-      <c r="B13">
-        <v>10807</v>
-      </c>
-      <c r="C13">
-        <v>6871</v>
+      <c r="B13" s="1">
+        <v>10120</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2737</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1.5728423810216854</v>
+        <v>3.6974789915966388</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>25</v>
       </c>
-      <c r="B14">
-        <v>12737</v>
-      </c>
-      <c r="C14">
-        <v>8162</v>
+      <c r="B14" s="1">
+        <v>11270</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2750</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>1.5605243812790983</v>
+        <v>4.0981818181818186</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>27</v>
       </c>
-      <c r="B15">
-        <v>12569</v>
-      </c>
-      <c r="C15">
-        <v>7954</v>
+      <c r="B15" s="1">
+        <v>12650</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2818</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1.5802112144832789</v>
+        <v>4.4889992902767917</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>29</v>
       </c>
-      <c r="B16">
-        <v>13475</v>
-      </c>
-      <c r="C16">
-        <v>8414</v>
+      <c r="B16" s="1">
+        <v>12871</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3325</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1.6014975041597337</v>
+        <v>3.8709774436090227</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>31</v>
       </c>
-      <c r="B17">
-        <v>14079</v>
-      </c>
-      <c r="C17">
-        <v>8151</v>
+      <c r="B17" s="1">
+        <v>13893</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3352</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1.7272727272727273</v>
+        <v>4.1446897374701672</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>33</v>
       </c>
-      <c r="B18">
-        <v>15811</v>
-      </c>
-      <c r="C18">
-        <v>9438</v>
+      <c r="B18" s="1">
+        <v>15540</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3298</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>1.6752489934308117</v>
+        <v>4.7119466343238328</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>35</v>
       </c>
-      <c r="B19">
-        <v>16688</v>
-      </c>
-      <c r="C19">
-        <v>9531</v>
+      <c r="B19" s="1">
+        <v>16489</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3254</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>1.7509180568670655</v>
+        <v>5.0673017824216346</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>37</v>
       </c>
-      <c r="B20">
-        <v>17726</v>
-      </c>
-      <c r="C20">
-        <v>9668</v>
+      <c r="B20" s="1">
+        <v>17257</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2642</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>1.8334712453454696</v>
+        <v>6.5317940953822857</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>39</v>
       </c>
-      <c r="B21">
-        <v>16850</v>
-      </c>
-      <c r="C21">
-        <v>8964</v>
+      <c r="B21" s="1">
+        <v>18088</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3607</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>1.8797411869701026</v>
+        <v>5.0146936512337126</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>41</v>
       </c>
-      <c r="B22">
-        <v>19355</v>
-      </c>
-      <c r="C22">
-        <v>10724</v>
+      <c r="B22" s="1">
+        <v>19536</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2980</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>1.8048302872062663</v>
+        <v>6.5557046979865774</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>43</v>
       </c>
-      <c r="B23">
-        <v>21004</v>
-      </c>
-      <c r="C23">
-        <v>11529</v>
+      <c r="B23" s="1">
+        <v>20432</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3659</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>1.8218405759389367</v>
+        <v>5.5840393550150313</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>45</v>
       </c>
-      <c r="B24">
-        <v>20621</v>
-      </c>
-      <c r="C24">
-        <v>11133</v>
+      <c r="B24" s="1">
+        <v>20992</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3301</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>1.8522410850624271</v>
+        <v>6.359285065131778</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>47</v>
       </c>
-      <c r="B25">
-        <v>20707</v>
-      </c>
-      <c r="C25">
-        <v>10241</v>
+      <c r="B25" s="1">
+        <v>22349</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2959</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>2.0219705106923151</v>
+        <v>7.5528894896924639</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>49</v>
       </c>
-      <c r="B26">
-        <v>21818</v>
-      </c>
-      <c r="C26">
-        <v>10806</v>
+      <c r="B26" s="1">
+        <v>22542</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3422</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>2.0190634832500463</v>
+        <v>6.5873758036236119</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>51</v>
       </c>
-      <c r="B27">
-        <v>23965</v>
-      </c>
-      <c r="C27">
-        <v>12516</v>
+      <c r="B27" s="1">
+        <v>23582</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3477</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>1.9147491211249601</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
-        <v>53</v>
-      </c>
-      <c r="B28">
-        <v>23272</v>
-      </c>
-      <c r="C28">
-        <v>10970</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>2.1214220601640839</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
-        <v>57</v>
-      </c>
-      <c r="B29">
-        <v>29013</v>
-      </c>
-      <c r="C29">
-        <v>13255</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>2.1888344021124104</v>
+        <v>6.7822835777969512</v>
       </c>
     </row>
   </sheetData>
@@ -1831,6 +1816,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1842,17 +1828,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1860,10 +1845,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>326</v>
+        <v>413</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1871,10 +1856,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1116</v>
+        <v>1401</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1882,10 +1867,10 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1938</v>
+        <v>2214</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1893,10 +1878,10 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>2880</v>
+        <v>3322</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1904,10 +1889,10 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>3684</v>
+        <v>4334</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1915,10 +1900,10 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>4660</v>
+        <v>4879</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1926,10 +1911,10 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>5590</v>
+        <v>6104</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1937,10 +1922,10 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>6298</v>
+        <v>7546</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>5307</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1948,10 +1933,10 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>7107</v>
+        <v>8325</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>6095</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1959,10 +1944,10 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>8204</v>
+        <v>9177</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>5877</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1970,10 +1955,10 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>9108</v>
+        <v>10038</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>6754</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1981,10 +1966,10 @@
         <v>23</v>
       </c>
       <c r="B12">
-        <v>10277</v>
+        <v>10807</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>6871</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1992,10 +1977,10 @@
         <v>25</v>
       </c>
       <c r="B13">
-        <v>11065</v>
+        <v>12737</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>8162</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2003,10 +1988,10 @@
         <v>27</v>
       </c>
       <c r="B14">
-        <v>12180</v>
+        <v>12569</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>7954</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2014,10 +1999,10 @@
         <v>29</v>
       </c>
       <c r="B15">
-        <v>13383</v>
+        <v>13475</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>8414</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2025,10 +2010,10 @@
         <v>31</v>
       </c>
       <c r="B16">
-        <v>14086</v>
+        <v>14079</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>8151</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2036,10 +2021,10 @@
         <v>33</v>
       </c>
       <c r="B17">
-        <v>15069</v>
+        <v>15811</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>9438</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2047,10 +2032,10 @@
         <v>35</v>
       </c>
       <c r="B18">
-        <v>15774</v>
+        <v>16688</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>9531</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2058,10 +2043,10 @@
         <v>37</v>
       </c>
       <c r="B19">
-        <v>16835</v>
+        <v>17726</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>9668</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2069,10 +2054,10 @@
         <v>39</v>
       </c>
       <c r="B20">
-        <v>17777</v>
+        <v>16850</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>8964</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2080,10 +2065,10 @@
         <v>41</v>
       </c>
       <c r="B21">
-        <v>19021</v>
+        <v>19355</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>10724</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2091,10 +2076,10 @@
         <v>43</v>
       </c>
       <c r="B22">
-        <v>20261</v>
+        <v>21004</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>11529</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2102,10 +2087,10 @@
         <v>45</v>
       </c>
       <c r="B23">
-        <v>21659</v>
+        <v>20621</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>11133</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2113,10 +2098,10 @@
         <v>47</v>
       </c>
       <c r="B24">
-        <v>22531</v>
+        <v>20707</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>10241</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2124,32 +2109,43 @@
         <v>49</v>
       </c>
       <c r="B25">
-        <v>23547</v>
+        <v>21818</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>10806</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26">
-        <v>26029</v>
+        <v>23965</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>12516</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
+        <v>53</v>
+      </c>
+      <c r="B27">
+        <v>23272</v>
+      </c>
+      <c r="C27">
+        <v>10970</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
         <v>57</v>
       </c>
-      <c r="B27">
-        <v>26314</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
+      <c r="B28">
+        <v>29013</v>
+      </c>
+      <c r="C28">
+        <v>13255</v>
       </c>
     </row>
   </sheetData>
@@ -2163,4 +2159,341 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>409</v>
+      </c>
+      <c r="C1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1159</v>
+      </c>
+      <c r="C2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2110</v>
+      </c>
+      <c r="C3">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2838</v>
+      </c>
+      <c r="C4">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>3597</v>
+      </c>
+      <c r="C5">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>4496</v>
+      </c>
+      <c r="C6">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>5585</v>
+      </c>
+      <c r="C7">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>6411</v>
+      </c>
+      <c r="C8">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>7539</v>
+      </c>
+      <c r="C9">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>8529</v>
+      </c>
+      <c r="C10">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>9171</v>
+      </c>
+      <c r="C11">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>10120</v>
+      </c>
+      <c r="C12">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>11270</v>
+      </c>
+      <c r="C13">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>12650</v>
+      </c>
+      <c r="C14">
+        <v>2818</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>12871</v>
+      </c>
+      <c r="C15">
+        <v>3325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>13893</v>
+      </c>
+      <c r="C16">
+        <v>3352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>15540</v>
+      </c>
+      <c r="C17">
+        <v>3298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>16489</v>
+      </c>
+      <c r="C18">
+        <v>3254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>37</v>
+      </c>
+      <c r="B19">
+        <v>17257</v>
+      </c>
+      <c r="C19">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>18088</v>
+      </c>
+      <c r="C20">
+        <v>3607</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>19536</v>
+      </c>
+      <c r="C21">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>43</v>
+      </c>
+      <c r="B22">
+        <v>20432</v>
+      </c>
+      <c r="C22">
+        <v>3659</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>45</v>
+      </c>
+      <c r="B23">
+        <v>20992</v>
+      </c>
+      <c r="C23">
+        <v>3301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>47</v>
+      </c>
+      <c r="B24">
+        <v>22349</v>
+      </c>
+      <c r="C24">
+        <v>2959</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>22542</v>
+      </c>
+      <c r="C25">
+        <v>3422</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>51</v>
+      </c>
+      <c r="B26">
+        <v>23582</v>
+      </c>
+      <c r="C26">
+        <v>3477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>2649</v>
+      </c>
+      <c r="C27">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>55</v>
+      </c>
+      <c r="B28">
+        <v>11486</v>
+      </c>
+      <c r="C28">
+        <v>2947</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:C28">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>